<commit_message>
Implementation of ID tags in progress
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-CPU-0858\Desktop\Work Files\Other Work Files\Scripts &amp; Automation\Python Scripts\RSB Quantifier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\RSB Quantifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F2ADE0-1457-4117-8B55-DD338E19DB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E136821-1654-4019-8A0B-C12801A123A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LENGTHS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Lengths</t>
   </si>
@@ -44,6 +44,63 @@
   </si>
   <si>
     <t>Diameter</t>
+  </si>
+  <si>
+    <t>TagID</t>
+  </si>
+  <si>
+    <t>FloorID</t>
+  </si>
+  <si>
+    <t>ZoneID</t>
+  </si>
+  <si>
+    <t>LocationID</t>
+  </si>
+  <si>
+    <t>MemberTypeID</t>
+  </si>
+  <si>
+    <t>RebarTypeID</t>
+  </si>
+  <si>
+    <t>SpecificTagID</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -380,19 +437,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +464,29 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.8</v>
       </c>
@@ -413,8 +496,11 @@
       <c r="C2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.25</v>
       </c>
@@ -424,8 +510,11 @@
       <c r="C3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.5</v>
       </c>
@@ -435,8 +524,11 @@
       <c r="C4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10.5</v>
       </c>
@@ -446,8 +538,11 @@
       <c r="C5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -457,8 +552,11 @@
       <c r="C6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.9</v>
       </c>
@@ -468,8 +566,11 @@
       <c r="C7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2</v>
       </c>
@@ -479,8 +580,11 @@
       <c r="C8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -490,8 +594,11 @@
       <c r="C9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -501,8 +608,11 @@
       <c r="C10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.4000000000000004</v>
       </c>
@@ -512,8 +622,11 @@
       <c r="C11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3.2</v>
       </c>
@@ -523,8 +636,11 @@
       <c r="C12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -533,6 +649,9 @@
       </c>
       <c r="C13">
         <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>